<commit_message>
improved the graph visualization for model and transaction drawers
</commit_message>
<xml_diff>
--- a/data/577 Projects/COCOMO Estimations.xlsx
+++ b/data/577 Projects/COCOMO Estimations.xlsx
@@ -103,69 +103,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team01\team01b\Development\RCP</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team02\team02b\new\Final Deliverables</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team03\team03a\FinalDeliveries</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team04\team04a\team04a\Artifacts\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team05\team05a\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team06\team06a\team06a\DCR-ARB-Team06-Package\DCR-ARB-Team06-Package</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team02\team02a\team02a\FINAL DELIVERABLE\FINAL DELIVERABLE</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team05\team05a\team05a\dcr</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team06\team06a\team06\Foundations</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team08\team08a\team08a</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team09\team09a\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team11\team11a\team11a\DCP</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team13\team13a\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team14\team14a\Team14\Final Deliverables (FD)\System and Software Architecture Description</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team15\team15a\team15a\DP</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team01\team01b\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team07\team07b\team07\Development</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team04\team04b\team04b\Final Deliverables-S15b</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team10\team10a\Foundation</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team12\team12b\team12\FinalDeliverables</t>
-  </si>
-  <si>
-    <t>C:\Users\Kan Qi\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team03\team03a\[18] As Built Package</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -239,6 +176,69 @@
   </si>
   <si>
     <t>93…</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team01\team01b\Development\RCP</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team02\team02b\new\Final Deliverables</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team03\team03a\FinalDeliveries</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team04\team04a\team04a\Artifacts\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team05\team05a\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2015\projects\team06\team06a\team06a\DCR-ARB-Team06-Package\DCR-ARB-Team06-Package</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team02\team02a\team02a\FINAL DELIVERABLE\FINAL DELIVERABLE</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team05\team05a\team05a\dcr</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team06\team06a\team06\Foundations</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team08\team08a\team08a</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team09\team09a\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team11\team11a\team11a\DCP</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team13\team13a\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team14\team14a\Team14\Final Deliverables (FD)\System and Software Architecture Description</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team15\team15a\team15a\DP</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team01\team01b\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team07\team07b\team07\Development</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team04\team04b\team04b\Final Deliverables-S15b</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team10\team10a\Foundation</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team12\team12b\team12\FinalDeliverables</t>
+  </si>
+  <si>
+    <t>C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Repositories\577 projects\fall2014\projects\team03\team03a\[18] As Built Package</t>
   </si>
 </sst>
 </file>
@@ -604,11 +604,13 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="13" max="14" width="22" customWidth="1"/>
     <col min="15" max="15" width="21.7109375" customWidth="1"/>
@@ -635,61 +637,61 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -703,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -720,10 +722,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F3">
         <v>2468</v>
@@ -738,7 +740,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="K3">
         <v>0.6</v>
@@ -782,7 +784,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>1943</v>
@@ -797,7 +799,7 @@
         <v>3.66</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="K4">
         <v>0.5</v>
@@ -805,7 +807,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>630</v>
@@ -820,7 +822,7 @@
         <v>0.67</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="K5">
         <v>0.1</v>
@@ -837,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -851,7 +853,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -865,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -879,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -893,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -910,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -924,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -938,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -952,7 +954,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -966,7 +968,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -980,7 +982,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,7 +996,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1008,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,7 +1024,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,7 +1038,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1052,7 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1064,7 +1066,7 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,7 +1094,7 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,7 +1108,7 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>